<commit_message>
Coloquei nn dentro da tabela de entrega
</commit_message>
<xml_diff>
--- a/Res_nn.xlsx
+++ b/Res_nn.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACA\Assignment1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45DA3C9-0500-4E0A-A166-D8E9F9B3E56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA6FB3C-9C40-4F2B-B44B-F47483240DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{384FCCFE-0EE5-4DB3-BAEC-B16F0F28FCBB}"/>
+    <workbookView xWindow="5760" yWindow="2856" windowWidth="17280" windowHeight="8880" xr2:uid="{384FCCFE-0EE5-4DB3-BAEC-B16F0F28FCBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>Method</t>
   </si>
   <si>
-    <t>Plain</t>
-  </si>
-  <si>
     <t>Gaussian</t>
   </si>
   <si>
@@ -56,12 +53,6 @@
     <t>C.H</t>
   </si>
   <si>
-    <t>Accuracy/Kaggle</t>
-  </si>
-  <si>
-    <t>Accuracy/Train</t>
-  </si>
-  <si>
     <t>ROC</t>
   </si>
   <si>
@@ -87,13 +78,25 @@
   </si>
   <si>
     <t>Ensemble</t>
+  </si>
+  <si>
+    <t>Acc/K</t>
+  </si>
+  <si>
+    <t>Acc/T</t>
+  </si>
+  <si>
+    <t>Serial</t>
+  </si>
+  <si>
+    <t>Ft. selection?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,15 +105,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -118,7 +119,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -126,7 +126,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -134,19 +133,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
       <color rgb="FF202124"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -342,9 +332,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -359,72 +350,70 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -445,7 +434,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -741,178 +730,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE018E3-EE5A-4199-8C2C-1FD16484E9CE}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="5.77734375" style="1" customWidth="1"/>
+    <col min="7" max="12" width="6" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="J2" s="14">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="K2" s="14">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="L2" s="14">
+        <v>150</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="19">
+        <v>0.97</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="I3" s="20">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="J3" s="20">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="K3" s="20">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="L3" s="20">
+        <v>147</v>
+      </c>
+      <c r="M3" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="H2" s="11">
-        <v>0.97699999999999998</v>
-      </c>
-      <c r="I2" s="12">
-        <v>0.97699999999999998</v>
-      </c>
-      <c r="J2" s="12">
-        <v>0.97899999999999998</v>
-      </c>
-      <c r="K2" s="12">
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="L2" s="12">
-        <v>150</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>14</v>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="19">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="H4" s="26">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="L4" s="13">
+        <v>185</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="16">
-        <v>0.97</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0.96899999999999997</v>
-      </c>
-      <c r="I3" s="17">
-        <v>0.96899999999999997</v>
-      </c>
-      <c r="J3" s="17">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="K3" s="17">
-        <v>0.96499999999999997</v>
-      </c>
-      <c r="L3" s="17">
-        <v>147</v>
-      </c>
-      <c r="M3" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="16">
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="H4" s="23">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="19">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="H5" s="13">
         <v>0.98299999999999998</v>
       </c>
-      <c r="I4" s="11">
-        <v>0.98299999999999998</v>
-      </c>
-      <c r="J4" s="11">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="K4" s="11">
+      <c r="I5" s="20">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="J5" s="20">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="K5" s="20">
         <v>0.97799999999999998</v>
       </c>
-      <c r="L4" s="11">
-        <v>185</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="16">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="H5" s="11">
-        <v>0.98299999999999998</v>
-      </c>
-      <c r="I5" s="17">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="J5" s="17">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="K5" s="17">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="L5" s="17">
+      <c r="L5" s="20">
         <v>151</v>
       </c>
-      <c r="M5" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G13" s="27"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H15" s="26"/>
+      <c r="M5" s="21" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -926,137 +913,145 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5022440-123F-4FA4-9808-D7960864B152}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="6" width="5.33203125" customWidth="1"/>
+    <col min="7" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="19">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="I3" s="20">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="J3" s="20">
+        <v>0.98</v>
+      </c>
+      <c r="K3" s="20">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="L3" s="20">
+        <v>354</v>
+      </c>
+      <c r="M3" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="13" t="s">
-        <v>14</v>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="15" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="16">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0.97699999999999998</v>
-      </c>
-      <c r="I3" s="17">
-        <v>0.97699999999999998</v>
-      </c>
-      <c r="J3" s="17">
-        <v>0.98</v>
-      </c>
-      <c r="K3" s="17">
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="L3" s="17">
-        <v>354</v>
-      </c>
-      <c r="M3" s="18" t="s">
-        <v>15</v>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="21" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O21" s="27"/>
+    <row r="21" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O21" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Coloquei os CSV dos testes
</commit_message>
<xml_diff>
--- a/Res_nn.xlsx
+++ b/Res_nn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA6FB3C-9C40-4F2B-B44B-F47483240DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1C70F1-C847-40A2-BFDB-B39051511C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2856" windowWidth="17280" windowHeight="8880" xr2:uid="{384FCCFE-0EE5-4DB3-BAEC-B16F0F28FCBB}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{384FCCFE-0EE5-4DB3-BAEC-B16F0F28FCBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -332,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -350,9 +350,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -377,9 +374,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -415,6 +409,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,7 +742,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,20 +754,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="29"/>
+      <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
@@ -779,125 +788,125 @@
       <c r="L1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12">
+      <c r="F2" s="10"/>
+      <c r="G2" s="31">
         <v>0.98099999999999998</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <v>0.97699999999999998</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="12">
         <v>0.97699999999999998</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="12">
         <v>0.97899999999999998</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="12">
         <v>0.97399999999999998</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="12">
         <v>150</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="19">
+      <c r="A3" s="30"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="12">
         <v>0.97</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <v>0.96899999999999997</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="12">
         <v>0.96899999999999997</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="12">
         <v>0.97199999999999998</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="12">
         <v>0.96499999999999997</v>
       </c>
-      <c r="L3" s="20">
+      <c r="L3" s="12">
         <v>147</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="19">
+      <c r="A4" s="30"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="12">
         <v>0.99399999999999999</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="12">
         <v>0.98299999999999998</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <v>0.98299999999999998</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="12">
         <v>0.98799999999999999</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="12">
         <v>0.97799999999999998</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="12">
         <v>185</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="19">
+      <c r="A5" s="30"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="12">
         <v>0.98399999999999999</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>0.98299999999999998</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="12">
         <v>0.98199999999999998</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="12">
         <v>0.98599999999999999</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="12">
         <v>0.97799999999999998</v>
       </c>
-      <c r="L5" s="20">
+      <c r="L5" s="12">
         <v>151</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="19" t="s">
         <v>12</v>
       </c>
     </row>
@@ -969,84 +978,84 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="15" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="19">
+      <c r="A3" s="28"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="17">
         <v>0.98799999999999999</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <v>0.97699999999999998</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="18">
         <v>0.97699999999999998</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="18">
         <v>0.98</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="18">
         <v>0.97399999999999998</v>
       </c>
-      <c r="L3" s="20">
+      <c r="L3" s="18">
         <v>354</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="15" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="21" t="s">
+      <c r="A5" s="28"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>